<commit_message>
testing solution methods, start of dynamic firms with taxes solution
</commit_message>
<xml_diff>
--- a/checking_equations.xlsx
+++ b/checking_equations.xlsx
@@ -297,8 +297,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -347,7 +349,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -370,6 +372,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -392,6 +395,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1424,7 +1428,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1432,7 +1436,7 @@
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1446,7 +1450,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1460,7 +1464,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1474,7 +1478,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1482,7 +1486,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1490,7 +1494,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1504,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1521,7 +1525,7 @@
         <v>0.98507508434181168</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1535,7 +1539,7 @@
         <v>0.77800000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1551,8 +1555,12 @@
         <f>D$1*D$12*(((($B$5+D$2)/D$10)*(D$8^((1-D$3)/D$3)))^(-1*D$3))</f>
         <v>0.32466997141310111</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <f>SUM(B14:D14)</f>
+        <v>0.70920563459260744</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1561,7 +1569,7 @@
         <v>0.70920563459260744</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -1594,6 +1602,10 @@
         <f>(1-D$1)*D$12*(((($B$6)/D$10)*(D$8^((1-D$3)/D$3)))^(-1*D$3))</f>
         <v>0.45406994360958863</v>
       </c>
+      <c r="E18">
+        <f>SUM(B18:D18)</f>
+        <v>1.3714139978597566</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
@@ -1636,8 +1648,8 @@
         <v>72</v>
       </c>
       <c r="B26">
-        <f>1</f>
-        <v>1</v>
+        <f>E14</f>
+        <v>0.70920563459260744</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1654,19 +1666,19 @@
       </c>
       <c r="B28">
         <f>$B$26-B$16</f>
-        <v>0.51506121379087699</v>
+        <v>0.22426684838348437</v>
       </c>
       <c r="C28">
         <f>$B$26-C$16</f>
-        <v>0.45106318020341463</v>
+        <v>0.16026881479602206</v>
       </c>
       <c r="D28">
-        <f t="shared" ref="C28:D28" si="0">$B$26-D$16</f>
-        <v>0.61546433682049373</v>
+        <f>$B$26-D$16</f>
+        <v>0.32466997141310111</v>
       </c>
       <c r="E28">
         <f>SUM(B28:D28)</f>
-        <v>1.5815887308147853</v>
+        <v>0.70920563459260755</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1675,15 +1687,15 @@
       </c>
       <c r="B31">
         <f>(B$10*(((B$1*B$12)/B$28)^(1/B$3))*(B$8^((B$3-1)/B$3)))-B$2</f>
-        <v>9.1860305118250107E-2</v>
+        <v>0.77</v>
       </c>
       <c r="C31">
         <f>(C$10*(((C$1*C$12)/C$28)^(1/C$3))*(C$8^((C$3-1)/C$3)))-C$2</f>
-        <v>3.8638801269730599E-2</v>
+        <v>0.76999999999999968</v>
       </c>
       <c r="D31">
         <f>(D$10*(((D$1*D$12)/D$28)^(1/D$3))*(D$8^((D$3-1)/D$3)))-D$2</f>
-        <v>0.17793410501788584</v>
+        <v>0.77000000000000024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dynamic firm problem updated code
</commit_message>
<xml_diff>
--- a/checking_equations.xlsx
+++ b/checking_equations.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="97">
   <si>
     <t>xi</t>
   </si>
@@ -249,13 +251,76 @@
   </si>
   <si>
     <t>Note - total K here should sum to K_s</t>
+  </si>
+  <si>
+    <t>tau_b</t>
+  </si>
+  <si>
+    <t>tau_d</t>
+  </si>
+  <si>
+    <t>tau_g</t>
+  </si>
+  <si>
+    <t>delta_tau</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>q = p_k*((1-tau_d)/(1-tau_g))*(1+((1-delta_tau)*tau_b*delta_tau*(((r/(1-tau_g))+delta_tau)**(-1.0))))</t>
+  </si>
+  <si>
+    <t>k/x = gamma*((((1-tau_d)/(1-tau_g))*(1-tau_b)*(p/q))**epsilon)*(A**(epsilon-1))*(((r/(1-tau_g))+delta)**(-1*epsilon))</t>
+  </si>
+  <si>
+    <t>k/x</t>
+  </si>
+  <si>
+    <t>l/x</t>
+  </si>
+  <si>
+    <t>l/x = (1-gamma)*(A**(epsilon-1))*((p/w)**epsilon)</t>
+  </si>
+  <si>
+    <t>p = (w*l_over_x + ((r*q)/((1-tau_d)*(1-tau_b)))*k_over_x + (((1-(tau_b*(1-delta_tau)))*delta*p_k)/(1-tau_b))*k_over_x)</t>
+  </si>
+  <si>
+    <t>k_demand = (X/A)*(((gamma**(1/epsilon))+ (((1-gamma)**(1/epsilon))*(((1-gamma)/gamma)**((epsilon-1)/epsilon))*((((1-tau_g)/((1-tau_d)*(1-tau_b)))*(q/w)*((r/(1-tau_g))+delta))**((epsilon-1)/epsilon))))**(epsilon/(1-epsilon)))</t>
+  </si>
+  <si>
+    <t>l_demand = K*((1-gamma)/gamma)*(((q/w)*((r/(1-tau_g))+delta)*((1-tau_g)/((1-tau_d)*(1-tau_b))))**epsilon)</t>
+  </si>
+  <si>
+    <t>MPK</t>
+  </si>
+  <si>
+    <t>r error</t>
+  </si>
+  <si>
+    <t>r_error = (q*((r/(1-tau_g))+delta)) - (((1-tau_d)/(1-tau_g))*(1-tau_b)*p*MPK)</t>
+  </si>
+  <si>
+    <t>checking Z</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>Z = (((1-tau_d)/(1-tau_g))*tau_b*delta_tau)/((r/(1-tau_g))+delta_tau)</t>
+  </si>
+  <si>
+    <t>ss r, w, T_H:  0.669505214586 1.00006616209 0.0545341105673</t>
+  </si>
+  <si>
+    <t>checking Z [ 0.03799848  0.04425294  0.05297201  0.04117253]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -279,6 +344,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -297,7 +369,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -345,11 +417,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -373,6 +500,33 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -396,6 +550,33 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1427,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1707,4 +1888,716 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E29" sqref="A10:E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.3</v>
+      </c>
+      <c r="C10">
+        <v>0.25</v>
+      </c>
+      <c r="D10">
+        <v>0.4</v>
+      </c>
+      <c r="E10">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.1</v>
+      </c>
+      <c r="C11">
+        <v>0.12</v>
+      </c>
+      <c r="D11">
+        <v>0.15</v>
+      </c>
+      <c r="E11">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C12">
+        <v>0.6</v>
+      </c>
+      <c r="D12">
+        <v>0.62</v>
+      </c>
+      <c r="E12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>1.2</v>
+      </c>
+      <c r="D19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>0.7</v>
+      </c>
+      <c r="C21">
+        <v>0.6</v>
+      </c>
+      <c r="D21">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E21">
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>1.05</v>
+      </c>
+      <c r="C23">
+        <v>1.22</v>
+      </c>
+      <c r="D23">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E23">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25">
+        <v>0.25</v>
+      </c>
+      <c r="C25">
+        <v>0.25</v>
+      </c>
+      <c r="D25">
+        <v>0.25</v>
+      </c>
+      <c r="E25">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29">
+        <f>B11*1.2</f>
+        <v>0.12</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:D29" si="0">C11*1.2</f>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29" si="1">E11*1.2</f>
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31">
+        <f>B23*((1-B26)/(1-B27))*(1+((1-B29)*B25*B29*((($B$14/(1-B27))+B29)^(-1))))</f>
+        <v>1.0811460674157305</v>
+      </c>
+      <c r="C31">
+        <f>C23*((1-C26)/(1-C27))*(1+((1-C29)*C25*C29*((($B$14/(1-C27))+C29)^(-1))))</f>
+        <v>1.26113295404814</v>
+      </c>
+      <c r="D31">
+        <f>D23*((1-D26)/(1-D27))*(1+((1-D29)*D25*D29*((($B$14/(1-D27))+D29)^(-1))))</f>
+        <v>1.1635031578947368</v>
+      </c>
+      <c r="E31">
+        <f>E23*((1-E26)/(1-E27))*(1+((1-E29)*E25*E29*((($B$14/(1-E27))+E29)^(-1))))</f>
+        <v>1.0327878536585364</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32">
+        <f>B10*((((1-B26)/(1-B27))*(1-B25)*(B19/B31))^B12)*(B17^(B12-1))*((($B$14/(1-B27))+B11)^(-1*B12))</f>
+        <v>0.2648701122114383</v>
+      </c>
+      <c r="C32">
+        <f>C10*((((1-C26)/(1-C27))*(1-C25)*(C19/C31))^C12)*(C17^(C12-1))*((($B$14/(1-C27))+C11)^(-1*C12))</f>
+        <v>0.21897522731212993</v>
+      </c>
+      <c r="D32">
+        <f>D10*((((1-D26)/(1-D27))*(1-D25)*(D19/D31))^D12)*(D17^(D12-1))*((($B$14/(1-D27))+D11)^(-1*D12))</f>
+        <v>0.34035888741105647</v>
+      </c>
+      <c r="E32">
+        <f>E10*((((1-E26)/(1-E27))*(1-E25)*(E19/E31))^E12)*(E17^(E12-1))*((($B$14/(1-E27))+E11)^(-1*E12))</f>
+        <v>0.27605773940166467</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33">
+        <f>(1-B10)*(B17^(B12-1))*((B19/$B$15)^(B12))</f>
+        <v>0.68871186727093869</v>
+      </c>
+      <c r="C33">
+        <f>(1-C10)*(C17^(C12-1))*((C19/$B$15)^(C12))</f>
+        <v>0.82199216161439415</v>
+      </c>
+      <c r="D33">
+        <f>(1-D10)*(D17^(D12-1))*((D19/$B$15)^(D12))</f>
+        <v>0.62496491321532077</v>
+      </c>
+      <c r="E33">
+        <f>(1-E10)*(E17^(E12-1))*((E19/$B$15)^(E12))</f>
+        <v>0.61789968461060796</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <f>($B$15*B33)+((($B$14*B31)/((1-B26)*(1-B25)))*B32)+((((1-(B25*(1-B29)))*B11*B23)/(1-B25))*B32)</f>
+        <v>1.0322966738744053</v>
+      </c>
+      <c r="C34">
+        <f>($B$15*C33)+((($B$14*C31)/((1-C26)*(1-C25)))*C32)+((((1-(C25*(1-C29)))*C11*C23)/(1-C25))*C32)</f>
+        <v>1.1637697410830925</v>
+      </c>
+      <c r="D34">
+        <f>($B$15*D33)+((($B$14*D31)/((1-D26)*(1-D25)))*D32)+((((1-(D25*(1-D29)))*D11*D23)/(1-D25))*D32)</f>
+        <v>1.1108938420107861</v>
+      </c>
+      <c r="E34">
+        <f>($B$15*E33)+((($B$14*E31)/((1-E26)*(1-E25)))*E32)+((((1-(E25*(1-E29)))*E11*E23)/(1-E25))*E32)</f>
+        <v>0.9608828373794116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:D35" si="2">(B21/B17)*(((B10^(1/B12))+(((1-B10)^(1/B12))*(((B31/$B$15)*((1-B27)/((1-B25)*(1-B26)))*(($B$14/(1-B27))+B11))^(B12-1))*(((1-B10)/B10)^((B12-1)/B12))))^(B12/(1-B12)))</f>
+        <v>0.19486883724679488</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>0.12719650560224116</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>0.2764773621960776</v>
+      </c>
+      <c r="E35">
+        <f>(E21/E17)*(((E10^(1/E12))+(((1-E10)^(1/E12))*(((E31/$B$15)*((1-E27)/((1-E25)*(1-E26)))*(($B$14/(1-E27))+E11))^(E12-1))*(((1-E10)/E10)^((E12-1)/E12))))^(E12/(1-E12)))</f>
+        <v>0.24066941189896141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <f>B35*((1-B10)/B10)*((($B$14/(1-B27))+B11)^(B12))*((B31/$B$15)^(B12))*(((1-B27)/((1-B25)*(1-B26)))^B12)</f>
+        <v>0.50669545028176655</v>
+      </c>
+      <c r="C36">
+        <f>C35*((1-C10)/C10)*((($B$14/(1-C27))+C11)^(C12))*((C31/$B$15)^(C12))*(((1-C27)/((1-C25)*(1-C26)))^C12)</f>
+        <v>0.47747195823548727</v>
+      </c>
+      <c r="D36">
+        <f>D35*((1-D10)/D10)*((($B$14/(1-D27))+D11)^(D12))*((D31/$B$15)^(D12))*(((1-D27)/((1-D25)*(1-D26)))^D12)</f>
+        <v>0.50766604622900025</v>
+      </c>
+      <c r="E36">
+        <f>E35*((1-E10)/E10)*((($B$14/(1-E27))+E11)^(E12))*((E31/$B$15)^(E12))*(((1-E27)/((1-E25)*(1-E26)))^E12)</f>
+        <v>0.53869003647608671</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37">
+        <f>(((B10*B21)/B35)^(1/B12))*(B17^((B12-1)/B12))</f>
+        <v>1.1456419578491084</v>
+      </c>
+      <c r="C37">
+        <f>(((C10*C21)/C35)^(1/C12))*(C17^((C12-1)/C12))</f>
+        <v>1.3163159119222749</v>
+      </c>
+      <c r="D37">
+        <f>(((D10*D21)/D35)^(1/D12))*(D17^((D12-1)/D12))</f>
+        <v>1.2102385583170632</v>
+      </c>
+      <c r="E37">
+        <f>(((E10*E21)/E35)^(1/E12))*(E17^((E12-1)/E12))</f>
+        <v>1.1137500423837636</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38">
+        <f>(B31*(($B$14/(1-B27))+B11)) - (((1-B26)/(1-B27))*(1-B25)*B19*B37)</f>
+        <v>8.1365610264854227E-2</v>
+      </c>
+      <c r="C38">
+        <f>(C31*(($B$14/(1-C27))+C11)) - (((1-C26)/(1-C27))*(1-C25)*C19*C37)</f>
+        <v>-6.2275991627202654E-2</v>
+      </c>
+      <c r="D38">
+        <f>(D31*(($B$14/(1-D27))+D11)) - (((1-D26)/(1-D27))*(1-D25)*D19*D37)</f>
+        <v>7.1976094651580724E-2</v>
+      </c>
+      <c r="E38">
+        <f>(E31*(($B$14/(1-E27))+E11)) - (((1-E26)/(1-E27))*(1-E25)*E19*E37)</f>
+        <v>0.15707203261047153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.3</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+      <c r="D7">
+        <v>0.4</v>
+      </c>
+      <c r="E7">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>0.12</v>
+      </c>
+      <c r="D8">
+        <v>0.15</v>
+      </c>
+      <c r="E8">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C9">
+        <v>0.6</v>
+      </c>
+      <c r="D9">
+        <v>0.62</v>
+      </c>
+      <c r="E9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0.66950521458599999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1.00006616209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1.2</v>
+      </c>
+      <c r="D16">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>0.7</v>
+      </c>
+      <c r="C18">
+        <v>0.6</v>
+      </c>
+      <c r="D18">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="E18">
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>1.05</v>
+      </c>
+      <c r="C20">
+        <v>1.22</v>
+      </c>
+      <c r="D20">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E20">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22">
+        <v>0.25</v>
+      </c>
+      <c r="C22">
+        <v>0.25</v>
+      </c>
+      <c r="D22">
+        <v>0.25</v>
+      </c>
+      <c r="E22">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26">
+        <f>B8*1.2</f>
+        <v>0.12</v>
+      </c>
+      <c r="C26">
+        <f t="shared" ref="C26:E26" si="0">C8*1.2</f>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>0.13200000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29">
+        <f>(((1-B23)/(1-B24))*B22*B26)/(($B$11/(1-B24))+B26)</f>
+        <v>3.799848239853789E-2</v>
+      </c>
+      <c r="C29">
+        <f>(((1-C23)/(1-C24))*C22*C26)/(($B$11/(1-C24))+C26)</f>
+        <v>4.425294313364754E-2</v>
+      </c>
+      <c r="D29">
+        <f>(((1-D23)/(1-D24))*D22*D26)/(($B$11/(1-D24))+D26)</f>
+        <v>5.2972011504285363E-2</v>
+      </c>
+      <c r="E29">
+        <f>(((1-E23)/(1-E24))*E22*E26)/(($B$11/(1-E24))+E26)</f>
+        <v>4.1172533128241005E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
One firm problem with Rex's code
</commit_message>
<xml_diff>
--- a/checking_equations.xlsx
+++ b/checking_equations.xlsx
@@ -2323,47 +2323,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:9">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2397,7 +2397,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>0.66950521458599999</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2430,7 +2430,13 @@
         <v>1.00006616209</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="13" spans="1:9">
+      <c r="I13">
+        <f>1.1^0.3</f>
+        <v>1.0290057594210951</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -2447,7 +2453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>41</v>
       </c>

</xml_diff>